<commit_message>
Levels ----- Completed Level 1
</commit_message>
<xml_diff>
--- a/Base/TileMap/Level1.xlsx
+++ b/Base/TileMap/Level1.xlsx
@@ -12,40 +12,52 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="Level0" sheetId="1" r:id="rId1"/>
+    <sheet name="Level1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>//1</t>
   </si>
   <si>
-    <t>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1</t>
+    <t>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1</t>
   </si>
   <si>
-    <t>1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1</t>
+    <t>1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1</t>
   </si>
   <si>
-    <t>1,-1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1</t>
+    <t>1,0,0,0,1,1,1,1,1,1,1,1,13,0,0,0,1,1,1,13,0,0,0,1,1</t>
   </si>
   <si>
-    <t>1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,0,0,15</t>
+    <t>1,0,-1,0,1,1,1,1,1,1,1,1,11,0,0,0,1,1,1,11,0,0,0,1,1</t>
   </si>
   <si>
-    <t>1,0,26,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1</t>
+    <t>1,0,0,0,1,1,1,1,1,1,1,1,13,4,0,0,1,1,1,13,4,0,0,1,1</t>
   </si>
   <si>
-    <t>1,0,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1</t>
+    <t>1,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,1,1,1,0,0,0,0,1,1</t>
   </si>
   <si>
-    <t>1,1,1,1,1,1,22,1,1,1,14,1,1,1,1,1,1,1,0,0,1</t>
+    <t>1,0,0,0,1,1,1,1,1,1,1,1,11,4,0,0,1,1,1,11,4,0,0,1,1</t>
   </si>
   <si>
-    <t>1,0,0,0,1,1,1,1,16,1,1,1,1,1,22,1,1,1,1,1,1</t>
+    <t>1,0,0,0,22,1,1,1,22,1,1,1,22,1,1,0,1,14,1,22,1,1,0,1,1</t>
+  </si>
+  <si>
+    <t>1,0,0,0,1,1,1,1,1,1,1,1,0,0,0,22,1,1,1,0,0,0,22,1,1</t>
+  </si>
+  <si>
+    <t>1,0,26,0,1,1,1,1,1,1,1,1,0,0,0,22,1,1,1,23,0,0,22,1,1</t>
+  </si>
+  <si>
+    <t>1,0,0,0,22,1,1,1,22,1,1,1,22,1,1,0,1,16,1,22,1,1,0,1,1</t>
+  </si>
+  <si>
+    <t>1,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,15,1,1</t>
   </si>
 </sst>
 </file>
@@ -194,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +392,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -541,12 +577,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -871,7 +912,7 @@
   <dimension ref="A1:BM48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:BM1"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1113,7 @@
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1083,29 +1124,29 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1116,32 +1157,32 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" s="3">
-        <v>0</v>
-      </c>
-      <c r="U3" s="3">
-        <v>0</v>
-      </c>
-      <c r="V3" s="3">
-        <v>0</v>
-      </c>
-      <c r="W3" s="3">
-        <v>0</v>
-      </c>
-      <c r="X3" s="3">
-        <v>0</v>
+      <c r="P3" s="9">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="9">
+        <v>22</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1</v>
       </c>
       <c r="Y3" s="1">
         <v>1</v>
@@ -1189,43 +1230,43 @@
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1236,29 +1277,29 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0</v>
-      </c>
-      <c r="X4" s="3">
-        <v>0</v>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>11</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1</v>
       </c>
       <c r="Y4" s="1">
         <v>1</v>
@@ -1306,10 +1347,10 @@
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1317,35 +1358,35 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1353,29 +1394,29 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0</v>
-      </c>
-      <c r="X5" s="3">
-        <v>0</v>
+      <c r="Q5" s="1">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>13</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
       </c>
       <c r="Y5" s="1">
         <v>1</v>
@@ -1423,7 +1464,7 @@
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1434,29 +1475,29 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1470,29 +1511,29 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0</v>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
       </c>
       <c r="Y6" s="1">
         <v>1</v>
@@ -1540,7 +1581,7 @@
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1551,29 +1592,29 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1587,29 +1628,29 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" s="3">
-        <v>0</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
-        <v>0</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0</v>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1</v>
       </c>
       <c r="Y7" s="1">
         <v>1</v>
@@ -1657,7 +1698,7 @@
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1668,29 +1709,29 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
       </c>
       <c r="M8" s="3">
         <v>0</v>
@@ -1704,14 +1745,14 @@
       <c r="P8" s="3">
         <v>0</v>
       </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
-      <c r="S8" s="3">
-        <v>0</v>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
       </c>
       <c r="T8" s="3">
         <v>0</v>
@@ -1725,8 +1766,8 @@
       <c r="W8" s="3">
         <v>0</v>
       </c>
-      <c r="X8" s="3">
-        <v>0</v>
+      <c r="X8" s="1">
+        <v>1</v>
       </c>
       <c r="Y8" s="1">
         <v>1</v>
@@ -1774,7 +1815,7 @@
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1785,29 +1826,29 @@
       <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
       </c>
       <c r="M9" s="3">
         <v>0</v>
@@ -1821,14 +1862,14 @@
       <c r="P9" s="3">
         <v>0</v>
       </c>
-      <c r="Q9" s="3">
-        <v>0</v>
-      </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="3">
-        <v>0</v>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1</v>
       </c>
       <c r="T9" s="3">
         <v>0</v>
@@ -1842,8 +1883,8 @@
       <c r="W9" s="3">
         <v>0</v>
       </c>
-      <c r="X9" s="3">
-        <v>0</v>
+      <c r="X9" s="1">
+        <v>1</v>
       </c>
       <c r="Y9" s="1">
         <v>1</v>
@@ -1891,7 +1932,7 @@
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -1902,29 +1943,29 @@
       <c r="D10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
       </c>
       <c r="M10" s="3">
         <v>0</v>
@@ -1938,14 +1979,14 @@
       <c r="P10" s="3">
         <v>0</v>
       </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="3">
-        <v>0</v>
-      </c>
-      <c r="S10" s="3">
-        <v>0</v>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>1</v>
       </c>
       <c r="T10" s="3">
         <v>0</v>
@@ -1959,8 +2000,8 @@
       <c r="W10" s="3">
         <v>0</v>
       </c>
-      <c r="X10" s="3">
-        <v>0</v>
+      <c r="X10" s="1">
+        <v>1</v>
       </c>
       <c r="Y10" s="1">
         <v>1</v>
@@ -2008,7 +2049,7 @@
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -2019,65 +2060,65 @@
       <c r="D11" s="3">
         <v>0</v>
       </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3">
-        <v>0</v>
+      <c r="E11" s="6">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>22</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6">
+        <v>22</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
       </c>
       <c r="P11" s="3">
         <v>0</v>
       </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3">
-        <v>0</v>
-      </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
-      <c r="T11" s="3">
-        <v>0</v>
-      </c>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
-      <c r="V11" s="3">
-        <v>0</v>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="7">
+        <v>14</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="6">
+        <v>22</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
       </c>
       <c r="W11" s="3">
         <v>0</v>
       </c>
-      <c r="X11" s="3">
-        <v>0</v>
+      <c r="X11" s="1">
+        <v>1</v>
       </c>
       <c r="Y11" s="1">
         <v>1</v>
@@ -2194,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12" s="1">
         <v>1</v>
@@ -2311,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="1">
         <v>1</v>
@@ -2359,7 +2400,7 @@
     </row>
     <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -2427,8 +2468,8 @@
       <c r="W14" s="3">
         <v>0</v>
       </c>
-      <c r="X14" s="3">
-        <v>0</v>
+      <c r="X14" s="7">
+        <v>15</v>
       </c>
       <c r="Y14" s="1">
         <v>1</v>
@@ -2476,7 +2517,7 @@
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -2545,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="1">
         <v>1</v>
@@ -2593,7 +2634,7 @@
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -2628,13 +2669,13 @@
       <c r="L16" s="3">
         <v>0</v>
       </c>
-      <c r="M16" s="3">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3">
-        <v>0</v>
-      </c>
-      <c r="O16" s="3">
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
         <v>0</v>
       </c>
       <c r="P16" s="3">
@@ -2649,20 +2690,20 @@
       <c r="S16" s="3">
         <v>0</v>
       </c>
-      <c r="T16" s="3">
-        <v>0</v>
-      </c>
-      <c r="U16" s="3">
-        <v>0</v>
-      </c>
-      <c r="V16" s="3">
+      <c r="T16" s="5">
+        <v>0</v>
+      </c>
+      <c r="U16" s="5">
+        <v>0</v>
+      </c>
+      <c r="V16" s="5">
         <v>0</v>
       </c>
       <c r="W16" s="3">
         <v>0</v>
       </c>
       <c r="X16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="1">
         <v>1</v>
@@ -2710,7 +2751,7 @@
     </row>
     <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -2721,65 +2762,65 @@
       <c r="D17" s="3">
         <v>0</v>
       </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>0</v>
-      </c>
-      <c r="N17" s="3">
-        <v>0</v>
-      </c>
-      <c r="O17" s="3">
-        <v>0</v>
+      <c r="E17" s="6">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6">
+        <v>22</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6">
+        <v>22</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
+        <v>1</v>
       </c>
       <c r="P17" s="3">
         <v>0</v>
       </c>
-      <c r="Q17" s="3">
-        <v>0</v>
-      </c>
-      <c r="R17" s="3">
-        <v>0</v>
-      </c>
-      <c r="S17" s="3">
-        <v>0</v>
-      </c>
-      <c r="T17" s="3">
-        <v>0</v>
-      </c>
-      <c r="U17" s="3">
-        <v>0</v>
-      </c>
-      <c r="V17" s="3">
-        <v>0</v>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7">
+        <v>16</v>
+      </c>
+      <c r="S17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17" s="6">
+        <v>22</v>
+      </c>
+      <c r="U17" s="1">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1">
+        <v>1</v>
       </c>
       <c r="W17" s="3">
         <v>0</v>
       </c>
-      <c r="X17" s="3">
-        <v>0</v>
+      <c r="X17" s="1">
+        <v>1</v>
       </c>
       <c r="Y17" s="1">
         <v>1</v>
@@ -2838,29 +2879,29 @@
       <c r="D18" s="3">
         <v>0</v>
       </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
       </c>
       <c r="M18" s="3">
         <v>0</v>
@@ -2869,19 +2910,19 @@
         <v>0</v>
       </c>
       <c r="O18" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P18" s="3">
         <v>0</v>
       </c>
-      <c r="Q18" s="3">
-        <v>0</v>
-      </c>
-      <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="3">
-        <v>0</v>
+      <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1</v>
       </c>
       <c r="T18" s="3">
         <v>0</v>
@@ -2890,13 +2931,13 @@
         <v>0</v>
       </c>
       <c r="V18" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W18" s="3">
         <v>0</v>
       </c>
-      <c r="X18" s="3">
-        <v>0</v>
+      <c r="X18" s="1">
+        <v>1</v>
       </c>
       <c r="Y18" s="1">
         <v>1</v>
@@ -2955,29 +2996,29 @@
       <c r="D19" s="3">
         <v>0</v>
       </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0</v>
-      </c>
-      <c r="L19" s="3">
-        <v>0</v>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
       </c>
       <c r="M19" s="3">
         <v>0</v>
@@ -2991,14 +3032,14 @@
       <c r="P19" s="3">
         <v>0</v>
       </c>
-      <c r="Q19" s="3">
-        <v>0</v>
-      </c>
-      <c r="R19" s="3">
-        <v>0</v>
-      </c>
-      <c r="S19" s="3">
-        <v>0</v>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1</v>
       </c>
       <c r="T19" s="3">
         <v>0</v>
@@ -3012,8 +3053,8 @@
       <c r="W19" s="3">
         <v>0</v>
       </c>
-      <c r="X19" s="3">
-        <v>0</v>
+      <c r="X19" s="1">
+        <v>1</v>
       </c>
       <c r="Y19" s="1">
         <v>1</v>
@@ -3061,7 +3102,7 @@
     </row>
     <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>0</v>
@@ -3072,29 +3113,29 @@
       <c r="D20" s="3">
         <v>0</v>
       </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="3">
-        <v>0</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
       </c>
       <c r="M20" s="3">
         <v>0</v>
@@ -3108,14 +3149,14 @@
       <c r="P20" s="3">
         <v>0</v>
       </c>
-      <c r="Q20" s="3">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0</v>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1">
+        <v>1</v>
       </c>
       <c r="T20" s="3">
         <v>0</v>
@@ -3129,8 +3170,8 @@
       <c r="W20" s="3">
         <v>0</v>
       </c>
-      <c r="X20" s="3">
-        <v>0</v>
+      <c r="X20" s="1">
+        <v>1</v>
       </c>
       <c r="Y20" s="1">
         <v>1</v>
@@ -3178,7 +3219,7 @@
     </row>
     <row r="21" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3189,29 +3230,29 @@
       <c r="D21" s="3">
         <v>0</v>
       </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3">
-        <v>0</v>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
       </c>
       <c r="M21" s="3">
         <v>0</v>
@@ -3225,14 +3266,14 @@
       <c r="P21" s="3">
         <v>0</v>
       </c>
-      <c r="Q21" s="3">
-        <v>0</v>
-      </c>
-      <c r="R21" s="3">
-        <v>0</v>
-      </c>
-      <c r="S21" s="3">
-        <v>0</v>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1">
+        <v>1</v>
       </c>
       <c r="T21" s="3">
         <v>0</v>
@@ -3246,8 +3287,8 @@
       <c r="W21" s="3">
         <v>0</v>
       </c>
-      <c r="X21" s="3">
-        <v>0</v>
+      <c r="X21" s="1">
+        <v>1</v>
       </c>
       <c r="Y21" s="1">
         <v>1</v>
@@ -3295,7 +3336,7 @@
     </row>
     <row r="22" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -3306,29 +3347,29 @@
       <c r="D22" s="3">
         <v>0</v>
       </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3">
-        <v>0</v>
-      </c>
-      <c r="L22" s="3">
-        <v>0</v>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
       </c>
       <c r="M22" s="3">
         <v>0</v>
@@ -3342,14 +3383,14 @@
       <c r="P22" s="3">
         <v>0</v>
       </c>
-      <c r="Q22" s="3">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3">
-        <v>0</v>
-      </c>
-      <c r="S22" s="3">
-        <v>0</v>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>1</v>
       </c>
       <c r="T22" s="3">
         <v>0</v>
@@ -3363,8 +3404,8 @@
       <c r="W22" s="3">
         <v>0</v>
       </c>
-      <c r="X22" s="3">
-        <v>0</v>
+      <c r="X22" s="1">
+        <v>1</v>
       </c>
       <c r="Y22" s="1">
         <v>1</v>
@@ -3372,7 +3413,7 @@
     </row>
     <row r="23" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -3383,35 +3424,35 @@
       <c r="D23" s="3">
         <v>0</v>
       </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="L23" s="3">
-        <v>0</v>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
       </c>
       <c r="M23" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N23" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O23" s="3">
         <v>0</v>
@@ -3419,20 +3460,20 @@
       <c r="P23" s="3">
         <v>0</v>
       </c>
-      <c r="Q23" s="3">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3">
-        <v>0</v>
-      </c>
-      <c r="S23" s="3">
-        <v>0</v>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
+        <v>1</v>
       </c>
       <c r="T23" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="U23" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V23" s="3">
         <v>0</v>
@@ -3440,8 +3481,8 @@
       <c r="W23" s="3">
         <v>0</v>
       </c>
-      <c r="X23" s="3">
-        <v>0</v>
+      <c r="X23" s="1">
+        <v>1</v>
       </c>
       <c r="Y23" s="1">
         <v>1</v>
@@ -3449,7 +3490,7 @@
     </row>
     <row r="24" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -3460,32 +3501,32 @@
       <c r="D24" s="3">
         <v>0</v>
       </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3">
-        <v>0</v>
-      </c>
-      <c r="L24" s="3">
-        <v>0</v>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
       </c>
       <c r="M24" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
@@ -3496,17 +3537,17 @@
       <c r="P24" s="3">
         <v>0</v>
       </c>
-      <c r="Q24" s="3">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3">
-        <v>0</v>
-      </c>
-      <c r="S24" s="3">
-        <v>0</v>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>1</v>
       </c>
       <c r="T24" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="U24" s="3">
         <v>0</v>
@@ -3517,8 +3558,8 @@
       <c r="W24" s="3">
         <v>0</v>
       </c>
-      <c r="X24" s="3">
-        <v>0</v>
+      <c r="X24" s="1">
+        <v>1</v>
       </c>
       <c r="Y24" s="1">
         <v>1</v>
@@ -3526,40 +3567,40 @@
     </row>
     <row r="25" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
       </c>
-      <c r="C25" s="3">
-        <v>0</v>
+      <c r="C25" s="8">
+        <v>26</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" s="3">
-        <v>0</v>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
       </c>
       <c r="M25" s="3">
         <v>0</v>
@@ -3570,20 +3611,20 @@
       <c r="O25" s="3">
         <v>0</v>
       </c>
-      <c r="P25" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3">
-        <v>0</v>
-      </c>
-      <c r="R25" s="3">
-        <v>0</v>
-      </c>
-      <c r="S25" s="3">
-        <v>0</v>
+      <c r="P25" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1">
+        <v>1</v>
       </c>
       <c r="T25" s="3">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U25" s="3">
         <v>0</v>
@@ -3591,11 +3632,11 @@
       <c r="V25" s="3">
         <v>0</v>
       </c>
-      <c r="W25" s="3">
-        <v>0</v>
-      </c>
-      <c r="X25" s="3">
-        <v>0</v>
+      <c r="W25" s="6">
+        <v>22</v>
+      </c>
+      <c r="X25" s="1">
+        <v>1</v>
       </c>
       <c r="Y25" s="1">
         <v>1</v>

</xml_diff>